<commit_message>
Add feat message send,email validation
</commit_message>
<xml_diff>
--- a/email-service/BoardonSheetTest.xlsx
+++ b/email-service/BoardonSheetTest.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>First Name</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>Company</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
   <si>
     <t>Abhishek</t>
@@ -60,15 +63,15 @@
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="8.0"/>
       <color rgb="FF000000"/>
       <name val="&quot;Helvetica Neue&quot;"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,11 +109,11 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -341,40 +344,49 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>9.19167510548E11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <v>9.19167510548E11</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>